<commit_message>
corrected errors and double checked data
</commit_message>
<xml_diff>
--- a/cheese-database.xlsx
+++ b/cheese-database.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffan\Desktop\Intel Sys\Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="198"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="201">
   <si>
     <t>NAME</t>
   </si>
@@ -81,9 +76,6 @@
     <t>cow</t>
   </si>
   <si>
-    <t>england</t>
-  </si>
-  <si>
     <t>hard</t>
   </si>
   <si>
@@ -144,9 +136,6 @@
     <t>semi soft</t>
   </si>
   <si>
-    <t>springy, stringy, supple</t>
-  </si>
-  <si>
     <t>milky</t>
   </si>
   <si>
@@ -174,15 +163,9 @@
     <t>nutty, strong</t>
   </si>
   <si>
-    <t>asiago</t>
-  </si>
-  <si>
     <t>compact, crumbly, open, smooth</t>
   </si>
   <si>
-    <t>Full-flavoured, mild, milky, sharp</t>
-  </si>
-  <si>
     <t>mascarpone</t>
   </si>
   <si>
@@ -229,9 +212,6 @@
   </si>
   <si>
     <t>cottage cheese</t>
-  </si>
-  <si>
-    <t>united kingdom</t>
   </si>
   <si>
     <t>creamy, crumbly</t>
@@ -437,9 +417,6 @@
     <t>Weichkaese</t>
   </si>
   <si>
-    <t>soft,smare-ripened</t>
-  </si>
-  <si>
     <t>creamy,smooth</t>
   </si>
   <si>
@@ -452,9 +429,6 @@
     <t>belgium,germany,netherlands</t>
   </si>
   <si>
-    <t>semi-soft,smare-ripened</t>
-  </si>
-  <si>
     <t>creamy,crumbly,firm,smooth</t>
   </si>
   <si>
@@ -603,13 +577,64 @@
   </si>
   <si>
     <t>mild,savory,sharp</t>
+  </si>
+  <si>
+    <t>hard/artesian</t>
+  </si>
+  <si>
+    <t>hard/artesian/processed</t>
+  </si>
+  <si>
+    <t>soft/soft-ripened</t>
+  </si>
+  <si>
+    <t>full-flavored, mild, milky, sharp</t>
+  </si>
+  <si>
+    <t>soft/brined</t>
+  </si>
+  <si>
+    <t>Applewood</t>
+  </si>
+  <si>
+    <t>crumbly, dense</t>
+  </si>
+  <si>
+    <t>smokey</t>
+  </si>
+  <si>
+    <t>smokey, spicey</t>
+  </si>
+  <si>
+    <t>soft, processed</t>
+  </si>
+  <si>
+    <t>creamy, smooth</t>
+  </si>
+  <si>
+    <t>united kingdom, united states</t>
+  </si>
+  <si>
+    <t>soft/artesian/processed</t>
+  </si>
+  <si>
+    <t>medium firm, brined</t>
+  </si>
+  <si>
+    <t>semi soft/artesian/blue-veined</t>
+  </si>
+  <si>
+    <t>soft,smear-ripened</t>
+  </si>
+  <si>
+    <t>semi-soft,smear-ripened</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -618,6 +643,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -642,9 +673,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -917,7 +951,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -927,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -937,7 +971,7 @@
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.42578125"/>
     <col min="7" max="7" width="12.7109375"/>
     <col min="8" max="8" width="33.5703125"/>
@@ -950,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -982,7 +1016,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -991,7 +1025,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -1014,28 +1048,28 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="E3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
@@ -1043,7 +1077,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -1052,22 +1086,22 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>29</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
       </c>
       <c r="J4" t="s">
         <v>17</v>
@@ -1075,7 +1109,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -1084,22 +1118,22 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F5" t="s">
         <v>34</v>
       </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>35</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>36</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>37</v>
-      </c>
-      <c r="I5" t="s">
-        <v>38</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
@@ -1107,63 +1141,63 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>187</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="J6" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" t="s">
         <v>46</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
         <v>47</v>
       </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="I7" t="s">
         <v>48</v>
-      </c>
-      <c r="G7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" t="s">
-        <v>50</v>
       </c>
       <c r="J7" t="s">
         <v>17</v>
@@ -1171,66 +1205,66 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>193</v>
       </c>
       <c r="F8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" t="s">
         <v>52</v>
       </c>
-      <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" t="s">
-        <v>53</v>
-      </c>
       <c r="I8" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>185</v>
       </c>
       <c r="F9" t="s">
         <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H9" t="s">
         <v>56</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -1238,31 +1272,31 @@
         <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
       </c>
       <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>194</v>
+      </c>
+      <c r="G10" t="s">
         <v>58</v>
       </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>59</v>
       </c>
-      <c r="G10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>60</v>
       </c>
-      <c r="I10" t="s">
-        <v>25</v>
-      </c>
       <c r="J10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1270,31 +1304,31 @@
         <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
         <v>40</v>
       </c>
-      <c r="F11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" t="s">
-        <v>63</v>
-      </c>
       <c r="I11" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="J11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1302,118 +1336,118 @@
         <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
+        <v>195</v>
+      </c>
+      <c r="E12" t="s">
+        <v>196</v>
+      </c>
+      <c r="F12" t="s">
         <v>66</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" t="s">
         <v>67</v>
       </c>
-      <c r="F12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" t="s">
-        <v>42</v>
-      </c>
       <c r="I12" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="J12" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>197</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I13" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F14" t="s">
         <v>80</v>
       </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="G14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
         <v>81</v>
       </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>82</v>
       </c>
-      <c r="I14" t="s">
-        <v>83</v>
-      </c>
       <c r="J14" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" t="s">
         <v>84</v>
       </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" t="s">
-        <v>34</v>
-      </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>198</v>
       </c>
       <c r="F15" t="s">
         <v>85</v>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" t="s">
         <v>86</v>
@@ -1422,136 +1456,135 @@
         <v>87</v>
       </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="F16" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="G16" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H16" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="I16" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="J16" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D17" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H17" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I17" t="s">
-        <v>104</v>
+        <v>16</v>
       </c>
       <c r="J17" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" t="s">
         <v>108</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" t="s">
         <v>109</v>
       </c>
-      <c r="G18" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" t="s">
-        <v>110</v>
-      </c>
       <c r="I18" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" t="e">
-        <f>-20:20</f>
-        <v>#VALUE!</v>
+        <v>37</v>
+      </c>
+      <c r="J18" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
         <v>111</v>
       </c>
-      <c r="B19" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>112</v>
       </c>
-      <c r="D19" t="s">
-        <v>34</v>
-      </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
         <v>113</v>
       </c>
       <c r="G19" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H19" t="s">
         <v>114</v>
       </c>
       <c r="I19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J19" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1559,28 +1592,28 @@
         <v>115</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
         <v>116</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" t="s">
         <v>117</v>
       </c>
-      <c r="E20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" t="s">
-        <v>118</v>
-      </c>
-      <c r="G20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" t="s">
-        <v>119</v>
-      </c>
       <c r="I20" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="J20" t="s">
         <v>17</v>
@@ -1588,31 +1621,31 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" t="s">
         <v>120</v>
-      </c>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" t="s">
-        <v>116</v>
-      </c>
-      <c r="D21" t="s">
-        <v>58</v>
       </c>
       <c r="E21" t="s">
         <v>121</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="G21" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I21" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="J21" t="s">
         <v>17</v>
@@ -1620,31 +1653,31 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F22" t="s">
-        <v>127</v>
+        <v>55</v>
       </c>
       <c r="G22" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="H22" t="s">
         <v>128</v>
       </c>
       <c r="I22" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="J22" t="s">
         <v>17</v>
@@ -1652,31 +1685,31 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" t="s">
+        <v>199</v>
+      </c>
+      <c r="F23" t="s">
         <v>130</v>
       </c>
-      <c r="B23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="G23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" t="s">
         <v>131</v>
       </c>
-      <c r="E23" t="s">
-        <v>132</v>
-      </c>
-      <c r="F23" t="s">
-        <v>59</v>
-      </c>
-      <c r="G23" t="s">
-        <v>74</v>
-      </c>
-      <c r="H23" t="s">
-        <v>133</v>
-      </c>
       <c r="I23" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="J23" t="s">
         <v>17</v>
@@ -1684,31 +1717,31 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="E24" t="s">
+        <v>200</v>
+      </c>
+      <c r="F24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" t="s">
         <v>135</v>
       </c>
-      <c r="F24" t="s">
+      <c r="I24" t="s">
         <v>136</v>
-      </c>
-      <c r="G24" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" t="s">
-        <v>137</v>
-      </c>
-      <c r="I24" t="s">
-        <v>25</v>
       </c>
       <c r="J24" t="s">
         <v>17</v>
@@ -1716,159 +1749,159 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
         <v>19</v>
       </c>
       <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" t="s">
         <v>139</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" t="s">
         <v>140</v>
       </c>
-      <c r="F25" t="s">
+      <c r="I25" t="s">
         <v>141</v>
       </c>
-      <c r="G25" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" t="s">
-        <v>142</v>
-      </c>
-      <c r="I25" t="s">
-        <v>143</v>
-      </c>
       <c r="J25" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s">
         <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>143</v>
       </c>
       <c r="E26" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" t="s">
         <v>145</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
+        <v>69</v>
+      </c>
+      <c r="H26" t="s">
         <v>146</v>
       </c>
-      <c r="G26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>147</v>
       </c>
-      <c r="I26" t="s">
-        <v>148</v>
-      </c>
       <c r="J26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
         <v>19</v>
       </c>
       <c r="D27" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F27" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" t="s">
+        <v>71</v>
+      </c>
+      <c r="H27" t="s">
         <v>150</v>
       </c>
-      <c r="E27" t="s">
-        <v>151</v>
-      </c>
-      <c r="F27" t="s">
-        <v>152</v>
-      </c>
-      <c r="G27" t="s">
-        <v>74</v>
-      </c>
-      <c r="H27" t="s">
-        <v>153</v>
-      </c>
       <c r="I27" t="s">
-        <v>154</v>
+        <v>37</v>
       </c>
       <c r="J27" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C28" t="s">
         <v>19</v>
       </c>
       <c r="D28" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" t="s">
+        <v>153</v>
+      </c>
+      <c r="G28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H28" t="s">
+        <v>154</v>
+      </c>
+      <c r="I28" t="s">
         <v>156</v>
       </c>
-      <c r="F28" t="s">
-        <v>109</v>
-      </c>
-      <c r="G28" t="s">
-        <v>76</v>
-      </c>
-      <c r="H28" t="s">
-        <v>157</v>
-      </c>
-      <c r="I28" t="s">
-        <v>38</v>
-      </c>
       <c r="J28" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
         <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
+        <v>158</v>
+      </c>
+      <c r="G29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" t="s">
         <v>159</v>
       </c>
-      <c r="F29" t="s">
+      <c r="I29" t="s">
         <v>160</v>
-      </c>
-      <c r="G29" t="s">
-        <v>162</v>
-      </c>
-      <c r="H29" t="s">
-        <v>161</v>
-      </c>
-      <c r="I29" t="s">
-        <v>163</v>
       </c>
       <c r="J29" t="s">
         <v>17</v>
@@ -1876,31 +1909,31 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
         <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="E30" t="s">
-        <v>28</v>
+        <v>162</v>
       </c>
       <c r="F30" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G30" t="s">
         <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>166</v>
+        <v>67</v>
       </c>
       <c r="I30" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J30" t="s">
         <v>17</v>
@@ -1908,31 +1941,31 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
         <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="E31" t="s">
         <v>169</v>
       </c>
       <c r="F31" t="s">
+        <v>166</v>
+      </c>
+      <c r="G31" t="s">
+        <v>155</v>
+      </c>
+      <c r="H31" t="s">
+        <v>167</v>
+      </c>
+      <c r="I31" t="s">
         <v>170</v>
-      </c>
-      <c r="G31" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" t="s">
-        <v>72</v>
-      </c>
-      <c r="I31" t="s">
-        <v>171</v>
       </c>
       <c r="J31" t="s">
         <v>17</v>
@@ -1940,31 +1973,31 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" t="s">
+        <v>171</v>
+      </c>
+      <c r="G32" t="s">
+        <v>68</v>
+      </c>
+      <c r="H32" t="s">
         <v>172</v>
       </c>
-      <c r="B32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" t="s">
-        <v>176</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="I32" t="s">
         <v>173</v>
-      </c>
-      <c r="G32" t="s">
-        <v>162</v>
-      </c>
-      <c r="H32" t="s">
-        <v>174</v>
-      </c>
-      <c r="I32" t="s">
-        <v>177</v>
       </c>
       <c r="J32" t="s">
         <v>17</v>
@@ -1972,31 +2005,31 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>174</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
         <v>175</v>
       </c>
-      <c r="B33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" t="s">
-        <v>77</v>
-      </c>
-      <c r="D33" t="s">
-        <v>27</v>
-      </c>
       <c r="E33" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="F33" t="s">
+        <v>176</v>
+      </c>
+      <c r="G33" t="s">
+        <v>68</v>
+      </c>
+      <c r="H33" t="s">
         <v>178</v>
       </c>
-      <c r="G33" t="s">
-        <v>73</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>179</v>
-      </c>
-      <c r="I33" t="s">
-        <v>180</v>
       </c>
       <c r="J33" t="s">
         <v>17</v>
@@ -2004,71 +2037,71 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C34" t="s">
         <v>19</v>
       </c>
       <c r="D34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" t="s">
+        <v>181</v>
+      </c>
+      <c r="F34" t="s">
         <v>182</v>
       </c>
-      <c r="E34" t="s">
-        <v>184</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
+        <v>155</v>
+      </c>
+      <c r="H34" t="s">
         <v>183</v>
       </c>
-      <c r="G34" t="s">
-        <v>73</v>
-      </c>
-      <c r="H34" t="s">
-        <v>185</v>
-      </c>
       <c r="I34" t="s">
-        <v>186</v>
+        <v>16</v>
       </c>
       <c r="J34" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>187</v>
+      <c r="A35" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
         <v>19</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
+        <v>143</v>
       </c>
       <c r="E35" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="F35" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G35" t="s">
-        <v>162</v>
+        <v>14</v>
       </c>
       <c r="H35" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="I35" t="s">
-        <v>16</v>
+        <v>191</v>
       </c>
       <c r="J35" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>

</xml_diff>